<commit_message>
Fixed horizontal offset scrambling image. Fixed sub images being resized on cropping
</commit_message>
<xml_diff>
--- a/SpriteRipper/tiles.xlsx
+++ b/SpriteRipper/tiles.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicB\Documents\Visual Studio 2013\Projects\SpriteRipper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicB\Documents\Git\EnSys\SpriteRipper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Scratch" sheetId="2" r:id="rId1"/>
-    <sheet name="rpgmaker" sheetId="1" r:id="rId2"/>
+    <sheet name="Offset" sheetId="3" r:id="rId1"/>
+    <sheet name="Scratch" sheetId="2" r:id="rId2"/>
+    <sheet name="rpgmaker" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
   <si>
     <t>Width</t>
   </si>
@@ -68,13 +69,42 @@
   <si>
     <t>…</t>
   </si>
+  <si>
+    <t>Tile</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Cropped</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -182,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +245,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,9 +529,534 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="16" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+    </row>
+    <row r="3" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>256</v>
+      </c>
+      <c r="C5" s="1">
+        <v>211</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <f>H5*16</f>
+        <v>240</v>
+      </c>
+      <c r="G5" s="1">
+        <f>I5*16</f>
+        <v>192</v>
+      </c>
+      <c r="H5" s="1">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1">
+        <f>H5*I5</f>
+        <v>180</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <f>M5+16</f>
+        <v>20</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <f>M6+16</f>
+        <v>36</v>
+      </c>
+      <c r="N7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" ref="M8:M19" si="0">M7+16</f>
+        <v>52</v>
+      </c>
+      <c r="N8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="N9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="N10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <v>6</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="N11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <v>7</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="N12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="1">
+        <v>8</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="N13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="1">
+        <v>9</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="N14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L15" s="1">
+        <v>10</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="N15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L16" s="1">
+        <v>11</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="N16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="1">
+        <v>12</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="N17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="1">
+        <v>13</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+      <c r="N18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="1">
+        <v>14</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="N19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <v>15</v>
+      </c>
+      <c r="M20" s="1">
+        <v>4</v>
+      </c>
+      <c r="N20" s="1">
+        <f>N$5+16</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="1">
+        <v>16</v>
+      </c>
+      <c r="M21" s="1">
+        <f>M20+16</f>
+        <v>20</v>
+      </c>
+      <c r="N21" s="1">
+        <f>N$5+16</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="1">
+        <v>17</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" ref="M22:M35" si="1">M21+16</f>
+        <v>36</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" ref="N22:N35" si="2">N$5+16</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="1">
+        <v>18</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="1">
+        <v>19</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L25" s="1">
+        <v>20</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L26" s="1">
+        <v>21</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L27" s="1">
+        <v>22</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L28" s="1">
+        <v>23</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L29" s="1">
+        <v>24</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L30" s="1">
+        <v>25</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="1">
+        <v>26</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L32" s="1">
+        <v>27</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="1">
+        <v>28</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="1">
+        <v>29</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="1">
+        <v>30</v>
+      </c>
+      <c r="M35" s="1">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1">
+        <f>N$20+16</f>
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2621,7 +3180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AX147"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed incorrect subimages being displayed when subimage index is odd and greater than 1
</commit_message>
<xml_diff>
--- a/SpriteRipper/tiles.xlsx
+++ b/SpriteRipper/tiles.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Offset" sheetId="3" r:id="rId1"/>
     <sheet name="Scratch" sheetId="2" r:id="rId2"/>
     <sheet name="rpgmaker" sheetId="1" r:id="rId3"/>
+    <sheet name="288x864" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
   <si>
     <t>Width</t>
   </si>
@@ -89,6 +90,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -531,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,11 +874,11 @@
         <v>17</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" ref="M22:M35" si="1">M21+16</f>
+        <f t="shared" ref="M22:M34" si="1">M21+16</f>
         <v>36</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" ref="N22:N35" si="2">N$5+16</f>
+        <f t="shared" ref="N22:N34" si="2">N$5+16</f>
         <v>22</v>
       </c>
     </row>
@@ -9201,4 +9205,1903 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:S105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="9.140625" style="1"/>
+    <col min="17" max="18" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>288</v>
+      </c>
+      <c r="C5" s="1">
+        <v>864</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <f>D5*E5</f>
+        <v>8</v>
+      </c>
+      <c r="G5" s="1">
+        <f>B5/32</f>
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <f>C5/32</f>
+        <v>27</v>
+      </c>
+      <c r="I5" s="1">
+        <f>G5*H5</f>
+        <v>243</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>160</v>
+      </c>
+      <c r="M5" s="1">
+        <v>224</v>
+      </c>
+      <c r="N5" s="1">
+        <f>L5/32</f>
+        <v>5</v>
+      </c>
+      <c r="O5" s="1">
+        <f>M5/32</f>
+        <v>7</v>
+      </c>
+      <c r="P5" s="1">
+        <f>N5*O5</f>
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>MOD(K5,D$5)*L$5</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <f>INT(K5/D$5)*M$5</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <f>B$5-L5</f>
+        <v>128</v>
+      </c>
+      <c r="M6" s="1">
+        <f>M5</f>
+        <v>224</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N12" si="0">L6/32</f>
+        <v>4</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" ref="O6:O12" si="1">M6/32</f>
+        <v>7</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" ref="P6:P12" si="2">N6*O6</f>
+        <v>28</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ref="Q6:Q12" si="3">MOD(K6,D$5)*L$5</f>
+        <v>160</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" ref="R6:R12" si="4">INT(K6/D$5)*M$5</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1">
+        <f>L5</f>
+        <v>160</v>
+      </c>
+      <c r="M7" s="1">
+        <f>M6</f>
+        <v>224</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="4"/>
+        <v>224</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8" si="5">B$5-L7</f>
+        <v>128</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" ref="M8:M10" si="6">M7</f>
+        <v>224</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="4"/>
+        <v>224</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" ref="L9" si="7">L7</f>
+        <v>160</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="6"/>
+        <v>224</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="4"/>
+        <v>448</v>
+      </c>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10" si="8">B$5-L9</f>
+        <v>128</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="6"/>
+        <v>224</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="4"/>
+        <v>448</v>
+      </c>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" ref="L11" si="9">L9</f>
+        <v>160</v>
+      </c>
+      <c r="M11" s="1">
+        <f>C$5-M$5*(E$5-1)</f>
+        <v>192</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="4"/>
+        <v>672</v>
+      </c>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>7</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" ref="L12" si="10">B$5-L11</f>
+        <v>128</v>
+      </c>
+      <c r="M12" s="1">
+        <f>C$5-M$5*(E$5-1)</f>
+        <v>192</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="4"/>
+        <v>672</v>
+      </c>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18"/>
+      <c r="D18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="D19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="D20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="D21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="D22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73"/>
+      <c r="O73"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75"/>
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76"/>
+      <c r="O76"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77"/>
+      <c r="O77"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78"/>
+      <c r="O78"/>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79"/>
+      <c r="O79"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+      <c r="N83"/>
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
+      <c r="M84"/>
+      <c r="N84"/>
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85"/>
+      <c r="N85"/>
+      <c r="O85"/>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
+      <c r="M86"/>
+      <c r="N86"/>
+      <c r="O86"/>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
+      <c r="M88"/>
+      <c r="N88"/>
+      <c r="O88"/>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+      <c r="N92"/>
+      <c r="O92"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
+      <c r="N96"/>
+      <c r="O96"/>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B97"/>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
+      <c r="H97"/>
+      <c r="I97"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="L97"/>
+      <c r="M97"/>
+      <c r="N97"/>
+      <c r="O97"/>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B98"/>
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98"/>
+      <c r="M98"/>
+      <c r="N98"/>
+      <c r="O98"/>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B99"/>
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99"/>
+      <c r="M99"/>
+      <c r="N99"/>
+      <c r="O99"/>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B100"/>
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="L100"/>
+      <c r="M100"/>
+      <c r="N100"/>
+      <c r="O100"/>
+    </row>
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101"/>
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+    </row>
+    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102"/>
+      <c r="M102"/>
+      <c r="N102"/>
+      <c r="O102"/>
+    </row>
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
+      <c r="H103"/>
+      <c r="I103"/>
+      <c r="J103"/>
+      <c r="K103"/>
+      <c r="L103"/>
+      <c r="M103"/>
+      <c r="N103"/>
+      <c r="O103"/>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="L104"/>
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="L7:L11" formula="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>